<commit_message>
update dataset reference images
</commit_message>
<xml_diff>
--- a/doc/data/opentraj-datasets.xlsx
+++ b/doc/data/opentraj-datasets.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
   <si>
     <t>Sample</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Peds=786</t>
   </si>
   <si>
-    <t>![](PETS-2009/reference.png)</t>
+    <t>![](PETS-2009/reference.jpg)</t>
   </si>
   <si>
     <t>[PETS 2009](https://github.com/amiryanj/OpenTraj/blob/master/PETS-2009)</t>
@@ -111,7 +111,7 @@
     <t>8 top view scenes recorded by drone contains various types of agents</t>
   </si>
   <si>
-    <t>[website](http://cvgl.stanford.edu/projects/uav_data) [paper](http://svl.stanford.edu/assets/papers/ECCV16social.pdf)</t>
+    <t>[website](http://cvgl.stanford.edu/projects/uav_data) [paper](http://svl.stanford.edu/assets/papers/ECCV16social.pdf) [dropbox](https://www.dropbox.com/s/v9jvt4ln7t42m6m/StanfordDroneDataset.zip)</t>
   </si>
   <si>
     <t>Bikes=4210 Peds=5232 Skates=292 Carts=174 Cars=316 Buss=76 Total=10,300</t>
@@ -373,10 +373,10 @@
     <t>peds=1,200</t>
   </si>
   <si>
-    <t>![]</t>
-  </si>
-  <si>
-    <t>DUT</t>
+    <t>![](DUT/reference.png)</t>
+  </si>
+  <si>
+    <t>[DUT](https://github.com/amiryanj/OpenTraj/blob/master/DUT)</t>
   </si>
   <si>
     <t>Natural Vehicle-Crowd Interactions in crowded university campus</t>
@@ -388,7 +388,10 @@
     <t>Peds=1,739 vehicles=123 Total=1,862</t>
   </si>
   <si>
-    <t>CITR</t>
+    <t>![](CITR/reference.png)</t>
+  </si>
+  <si>
+    <t>[CITR](https://github.com/amiryanj/OpenTraj/blob/master/CITR)</t>
   </si>
   <si>
     <t>Fundamental Vehicle-Crowd Interaction scenarios in controlled experiments</t>
@@ -400,7 +403,10 @@
     <t>Peds=340</t>
   </si>
   <si>
-    <t>Ko-PER</t>
+    <t>![](Ko-PER/reference.png)</t>
+  </si>
+  <si>
+    <t>[Ko-PER](https://github.com/amiryanj/OpenTraj/blob/master/Ko-PER)</t>
   </si>
   <si>
     <t>Trajectories of People and vehicles at Urban Intersections (Laserscanner + Video)</t>
@@ -427,7 +433,10 @@
     <t>Cars=33 Bikes=20 Peds=11</t>
   </si>
   <si>
-    <t>ETH-Person</t>
+    <t>![](ETH-Person/reference.png)</t>
+  </si>
+  <si>
+    <t>[ETH-Person](https://github.com/amiryanj/OpenTraj/blob/master/ETH-Person)</t>
   </si>
   <si>
     <t>[website](https://data.vision.ee.ethz.ch/cvl/aess/)</t>
@@ -1444,19 +1453,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -1473,19 +1482,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -1496,19 +1505,19 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
@@ -1527,11 +1536,14 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed prediction benchmark tables
</commit_message>
<xml_diff>
--- a/doc/data/opentraj-datasets.xlsx
+++ b/doc/data/opentraj-datasets.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="144">
   <si>
     <t>Sample</t>
   </si>
@@ -41,10 +41,10 @@
     <t>Parser</t>
   </si>
   <si>
-    <t>![](ETH/seq_eth/reference.png)</t>
-  </si>
-  <si>
-    <t>[ETH](https://github.com/amiryanj/OpenTraj/blob/master/ETH)</t>
+    <t>![](datasets/ETH/seq_eth/reference.png)</t>
+  </si>
+  <si>
+    <t>[ETH](datasets/ETH)</t>
   </si>
   <si>
     <t>2 top view scenes containing walking pedestrians</t>
@@ -68,10 +68,10 @@
     <t>ParserETH</t>
   </si>
   <si>
-    <t>![](UCY/zara01/reference.png)</t>
-  </si>
-  <si>
-    <t>[UCY](https://github.com/amiryanj/OpenTraj/blob/master/UCY)</t>
+    <t>![](datasets/UCY/zara01/reference.png)</t>
+  </si>
+  <si>
+    <t>[UCY](datasets/UCY)</t>
   </si>
   <si>
     <t>3 scenes (Zara/Arxiepiskopi/University). Zara and University close to top view. Arxiepiskopi more inclined.</t>
@@ -84,10 +84,10 @@
     <t>Peds=786</t>
   </si>
   <si>
-    <t>![](PETS-2009/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[PETS 2009](https://github.com/amiryanj/OpenTraj/blob/master/PETS-2009)</t>
+    <t>![](datasets/PETS-2009/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[PETS 2009](datasets/PETS-2009)</t>
   </si>
   <si>
     <t>different crowd activities</t>
@@ -102,10 +102,10 @@
     <t>Not supported</t>
   </si>
   <si>
-    <t>![](SDD/coupa/video3/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[SDD](https://github.com/amiryanj/OpenTraj/blob/master/SDD)</t>
+    <t>![](datasets/SDD/coupa/video3/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[SDD](datasets/SDD)</t>
   </si>
   <si>
     <t>8 top view scenes recorded by drone contains various types of agents</t>
@@ -123,10 +123,10 @@
     <t>ParserSDD</t>
   </si>
   <si>
-    <t>![](GC/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[GC](https://github.com/amiryanj/OpenTraj/blob/master/GC)</t>
+    <t>![](datasets/GC/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[GC](datasets/GC)</t>
   </si>
   <si>
     <t>Grand Central Train Station Dataset: 1 scene of 33:20 minutes of crowd trajectories</t>
@@ -142,10 +142,10 @@
     <t>ParserGC</t>
   </si>
   <si>
-    <t>![](HERMES/reference.png)</t>
-  </si>
-  <si>
-    <t>[HERMES](https://github.com/amiryanj/OpenTraj/blob/master/HERMES)</t>
+    <t>![](datasets/HERMES/reference.png)</t>
+  </si>
+  <si>
+    <t>[HERMES](datasets/HERMES)</t>
   </si>
   <si>
     <t>Controlled Experiments of Pedestrian Dynamics (Unidirectional and bidirectional flows)</t>
@@ -160,10 +160,10 @@
     <t>ParserHermes</t>
   </si>
   <si>
-    <t>![](Waymo/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[Waymo](https://github.com/amiryanj/OpenTraj/blob/master/Waymo)</t>
+    <t>![](datasets/Waymo/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[Waymo](datasets/Waymo)</t>
   </si>
   <si>
     <t>High-resolution sensor data collected by Waymo self-driving cars</t>
@@ -178,10 +178,10 @@
     <t>self-driving car</t>
   </si>
   <si>
-    <t>![](KITTI/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[KITTI](https://github.com/amiryanj/OpenTraj/blob/master/KITTI)</t>
+    <t>![](datasets/KITTI/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[KITTI](datasets/KITTI)</t>
   </si>
   <si>
     <t>6 hours of traffic scenarios. various sensors</t>
@@ -193,10 +193,10 @@
     <t>image-3D + Calib</t>
   </si>
   <si>
-    <t>![](InD/reference.png)</t>
-  </si>
-  <si>
-    <t>[inD](https://github.com/amiryanj/OpenTraj/blob/master/InD)</t>
+    <t>![](datasets/InD/reference.png)</t>
+  </si>
+  <si>
+    <t>[inD](datasets/InD)</t>
   </si>
   <si>
     <t>Naturalistic Trajectories of Vehicles and Vulnerable Road Users Recorded at German Intersections</t>
@@ -208,10 +208,10 @@
     <t>Total=11,500</t>
   </si>
   <si>
-    <t>![](L-CAS/reference.png)</t>
-  </si>
-  <si>
-    <t>[L-CAS](https://github.com/amiryanj/OpenTraj/blob/master/L-CAS)</t>
+    <t>![](datasets/L-CAS/reference.png)</t>
+  </si>
+  <si>
+    <t>[L-CAS](datasets/L-CAS)</t>
   </si>
   <si>
     <t>Multisensor People Dataset Collected by a Pioneer 3-AT robot</t>
@@ -223,10 +223,10 @@
     <t>robot-view</t>
   </si>
   <si>
-    <t>![](VIRAT/reference.png)</t>
-  </si>
-  <si>
-    <t>[VIRAT](https://github.com/amiryanj/OpenTraj/blob/master/VIRAT)</t>
+    <t>![](datasets/VIRAT/reference.png)</t>
+  </si>
+  <si>
+    <t>[VIRAT](datasets/VIRAT)</t>
   </si>
   <si>
     <t>Natural scenes showing people performing normal actions</t>
@@ -235,10 +235,10 @@
     <t>[website](http://viratdata.org/)</t>
   </si>
   <si>
-    <t>![](VRU/reference.png)</t>
-  </si>
-  <si>
-    <t>[VRU](https://github.com/amiryanj/OpenTraj/blob/master/VRU)</t>
+    <t>![](datasets/VRU/reference.png)</t>
+  </si>
+  <si>
+    <t>[VRU](datasets/VRU)</t>
   </si>
   <si>
     <t>consists of pedestrian and cyclist trajectories, recorded at an urban intersection using cameras and LiDARs</t>
@@ -253,10 +253,10 @@
     <t>World (Meter)</t>
   </si>
   <si>
-    <t>![](Edinburgh/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[Edinburgh](https://github.com/amiryanj/OpenTraj/blob/master/Edinburgh)</t>
+    <t>![](datasets/Edinburgh/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[Edinburgh](datasets/Edinburgh)</t>
   </si>
   <si>
     <t>People walking through the Informatics Forum (University of Edinburgh)</t>
@@ -268,10 +268,10 @@
     <t>ped=+92,000</t>
   </si>
   <si>
-    <t>![](Town-Center/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[Town Center](https://github.com/amiryanj/OpenTraj/blob/master/Town-Center)</t>
+    <t>![](datasets/Town-Center/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[Town Center](datasets/Town-Center)</t>
   </si>
   <si>
     <t>CCTV video of pedestrians in a busy downtown area in Oxford</t>
@@ -283,10 +283,10 @@
     <t>peds=2,200</t>
   </si>
   <si>
-    <t>![](ATC/reference.png)</t>
-  </si>
-  <si>
-    <t>[ATC](https://github.com/amiryanj/OpenTraj/blob/master/ATC)</t>
+    <t>![](datasets/ATC/reference.png)</t>
+  </si>
+  <si>
+    <t>[ATC](datasets/ATC)</t>
   </si>
   <si>
     <t>92 days of pedestrian trajectories in a shopping center in Osaka, Japan</t>
@@ -298,10 +298,10 @@
     <t>world-2D + Range data</t>
   </si>
   <si>
-    <t>![](City-Scapes/reference.png)</t>
-  </si>
-  <si>
-    <t>[City Scapes](https://github.com/amiryanj/OpenTraj/blob/master/City-Scapes)</t>
+    <t>![](datasets/City-Scapes/reference.png)</t>
+  </si>
+  <si>
+    <t>[City Scapes](datasets/City-Scapes)</t>
   </si>
   <si>
     <t>25,000 annotated images (Semantic/ Instance-wise/ Dense pixel annotations)</t>
@@ -310,10 +310,10 @@
     <t>[website](https://www.cityscapes-dataset.com/dataset-overview/)</t>
   </si>
   <si>
-    <t>![](Forking-Paths-Garden/reference.png)</t>
-  </si>
-  <si>
-    <t>[Forking Paths Garden](https://github.com/amiryanj/OpenTraj/blob/master/Forking-Paths-Garden)</t>
+    <t>![](datasets/Forking-Paths-Garden/reference.png)</t>
+  </si>
+  <si>
+    <t>[Forking Paths Garden](datasets/Forking-Paths-Garden)</t>
   </si>
   <si>
     <t>**Multi-modal** _Synthetic_ dataset, created in [CARLA](https://carla.org) (3D simulator) based on real world trajectory data, extrapolated by human annotators</t>
@@ -322,10 +322,10 @@
     <t>[website](https://next.cs.cmu.edu/multiverse/index.html) [github](https://github.com/JunweiLiang/Multiverse) [paper](https://arxiv.org/abs/1912.06445)</t>
   </si>
   <si>
-    <t>![](NuScenes/reference.png)</t>
-  </si>
-  <si>
-    <t>[nuScenes](https://github.com/amiryanj/OpenTraj/blob/master/NuScenes)</t>
+    <t>![](datasets/NuScenes/reference.png)</t>
+  </si>
+  <si>
+    <t>[nuScenes](datasets/NuScenes)</t>
   </si>
   <si>
     <t>Large-scale Autonomous Driving dataset</t>
@@ -340,10 +340,10 @@
     <t>World + 3D Range Data</t>
   </si>
   <si>
-    <t>![](Argoverse/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[Argoverse](https://github.com/amiryanj/OpenTraj/blob/master/Argoverse)</t>
+    <t>![](datasets/Argoverse/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[Argoverse](datasets/Argoverse)</t>
   </si>
   <si>
     <t>320 hours of Self-driving dataset</t>
@@ -358,10 +358,10 @@
     <t>3D</t>
   </si>
   <si>
-    <t>![](Wild-Track/reference.jpg)</t>
-  </si>
-  <si>
-    <t>[Wild Track](https://github.com/amiryanj/OpenTraj/blob/master/Wild-Track)</t>
+    <t>![](datasets/Wild-Track/reference.jpg)</t>
+  </si>
+  <si>
+    <t>[Wild Track](datasets/Wild-Track)</t>
   </si>
   <si>
     <t>surveillance video dataset of students recorded outside the ETH university main building in Zurich.</t>
@@ -373,10 +373,10 @@
     <t>peds=1,200</t>
   </si>
   <si>
-    <t>![](DUT/reference.png)</t>
-  </si>
-  <si>
-    <t>[DUT](https://github.com/amiryanj/OpenTraj/blob/master/DUT)</t>
+    <t>![](datasets/DUT/reference.png)</t>
+  </si>
+  <si>
+    <t>[DUT](datasets/DUT)</t>
   </si>
   <si>
     <t>Natural Vehicle-Crowd Interactions in crowded university campus</t>
@@ -388,10 +388,10 @@
     <t>Peds=1,739 vehicles=123 Total=1,862</t>
   </si>
   <si>
-    <t>![](CITR/reference.png)</t>
-  </si>
-  <si>
-    <t>[CITR](https://github.com/amiryanj/OpenTraj/blob/master/CITR)</t>
+    <t>![](datasets/CITR/reference.png)</t>
+  </si>
+  <si>
+    <t>[CITR](datasets/CITR)</t>
   </si>
   <si>
     <t>Fundamental Vehicle-Crowd Interaction scenarios in controlled experiments</t>
@@ -403,10 +403,10 @@
     <t>Peds=340</t>
   </si>
   <si>
-    <t>![](Ko-PER/reference.png)</t>
-  </si>
-  <si>
-    <t>[Ko-PER](https://github.com/amiryanj/OpenTraj/blob/master/Ko-PER)</t>
+    <t>![](datasets/Ko-PER/reference.png)</t>
+  </si>
+  <si>
+    <t>[Ko-PER](datasets/Ko-PER)</t>
   </si>
   <si>
     <t>Trajectories of People and vehicles at Urban Intersections (Laserscanner + Video)</t>
@@ -418,10 +418,10 @@
     <t>peds=350</t>
   </si>
   <si>
-    <t>![](TRAF/reference.png)</t>
-  </si>
-  <si>
-    <t>[TRAF](https://github.com/amiryanj/OpenTraj/blob/master/TRAF)</t>
+    <t>![](datasets/TRAF/reference.png)</t>
+  </si>
+  <si>
+    <t>[TRAF](datasets/TRAF)</t>
   </si>
   <si>
     <t>small dataset of dense and heterogeneous traffic videos in India (22 footages)</t>
@@ -433,10 +433,13 @@
     <t>Cars=33 Bikes=20 Peds=11</t>
   </si>
   <si>
-    <t>![](ETH-Person/reference.png)</t>
-  </si>
-  <si>
-    <t>[ETH-Person](https://github.com/amiryanj/OpenTraj/blob/master/ETH-Person)</t>
+    <t>![](datasets/ETH-Person/reference.png)</t>
+  </si>
+  <si>
+    <t>[ETH-Person](datasets/ETH-Person)</t>
+  </si>
+  <si>
+    <t>Multi-Person Data Collected from Mobile Platforms</t>
   </si>
   <si>
     <t>[website](https://data.vision.ee.ethz.ch/cvl/aess/)</t>
@@ -1542,8 +1545,11 @@
       <c r="B26" t="s">
         <v>141</v>
       </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>